<commit_message>
macro formulated cells are modified for debugging in date conversion
</commit_message>
<xml_diff>
--- a/Test-Data/Example1.xlsx
+++ b/Test-Data/Example1.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tingas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilu\Navid\EA\EA-Heuristic\Test-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21622A45-1774-1E47-BE12-C011F97F55C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBE0B7C-7800-46EC-8CA9-74D34E825E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{2111CCAB-A59E-6343-8D75-11A7B1CA366B}"/>
+    <workbookView xWindow="3260" yWindow="3300" windowWidth="32310" windowHeight="16590" xr2:uid="{2111CCAB-A59E-6343-8D75-11A7B1CA366B}"/>
   </bookViews>
   <sheets>
     <sheet name="Aircraft_scheduling" sheetId="1" r:id="rId1"/>
     <sheet name="Work_packages" sheetId="2" r:id="rId2"/>
     <sheet name="Staff" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -432,7 +432,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -497,14 +497,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -849,11 +849,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7B622A-250F-6940-8572-A7F426096522}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="24" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="15.5" style="3" bestFit="1" customWidth="1"/>
@@ -863,7 +863,7 @@
     <col min="8" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>51</v>
       </c>
@@ -886,7 +886,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>101</v>
       </c>
@@ -911,7 +911,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>102</v>
@@ -937,7 +937,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A21" si="1">A3+1</f>
         <v>103</v>
@@ -963,7 +963,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -989,7 +989,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -1004,18 +1004,17 @@
         <v>45748</v>
       </c>
       <c r="E6" s="9">
-        <f>C6+0.181</f>
-        <v>0.64627777777777773</v>
+        <v>0.64627314814814818</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" si="0"/>
-        <v>0.18099999999999994</v>
+        <v>0.18099537037037039</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -1040,7 +1039,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -1065,7 +1064,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -1091,7 +1090,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -1117,7 +1116,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -1132,18 +1131,17 @@
         <v>45749</v>
       </c>
       <c r="E11" s="9">
-        <f>C11+0.556</f>
-        <v>1.2469722222222224</v>
+        <v>0.2469675925925926</v>
       </c>
       <c r="F11" s="9">
         <f t="shared" si="0"/>
-        <v>0.55600000000000016</v>
+        <v>0.55599537037037039</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -1158,8 +1156,7 @@
         <v>45749</v>
       </c>
       <c r="E12" s="9">
-        <f>C12+0.41</f>
-        <v>1.1322222222222222</v>
+        <v>0.13222222222222221</v>
       </c>
       <c r="F12" s="9">
         <f t="shared" si="0"/>
@@ -1169,7 +1166,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -1184,8 +1181,7 @@
         <v>45749</v>
       </c>
       <c r="E13" s="9">
-        <f>C13+0.5525</f>
-        <v>1.33375</v>
+        <v>0.33374999999999999</v>
       </c>
       <c r="F13" s="9">
         <f t="shared" si="0"/>
@@ -1195,7 +1191,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -1210,18 +1206,17 @@
         <v>45749</v>
       </c>
       <c r="E14" s="9">
-        <f>C14+0.6355</f>
-        <v>1.4306388888888888</v>
+        <v>0.43063657407407407</v>
       </c>
       <c r="F14" s="9">
         <f t="shared" si="0"/>
-        <v>0.63549999999999995</v>
+        <v>0.63549768518518523</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -1236,18 +1231,17 @@
         <v>45749</v>
       </c>
       <c r="E15" s="9">
-        <f>C15+0.455</f>
-        <v>1.2605555555555557</v>
+        <v>0.26055555555555554</v>
       </c>
       <c r="F15" s="9">
         <f t="shared" si="0"/>
-        <v>0.45500000000000007</v>
+        <v>0.45499999999999996</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -1262,18 +1256,17 @@
         <v>45749</v>
       </c>
       <c r="E16" s="9">
-        <f>C16+0.462</f>
-        <v>1.2918611111111111</v>
+        <v>0.29185185185185186</v>
       </c>
       <c r="F16" s="9">
         <f t="shared" si="0"/>
-        <v>0.46199999999999997</v>
+        <v>0.46199074074074065</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -1288,18 +1281,17 @@
         <v>45749</v>
       </c>
       <c r="E17" s="9">
-        <f>C17+0.511</f>
-        <v>1.3616944444444443</v>
+        <v>0.36168981481481483</v>
       </c>
       <c r="F17" s="9">
         <f t="shared" si="0"/>
-        <v>0.5109999999999999</v>
+        <v>0.51099537037037046</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -1314,18 +1306,17 @@
         <v>45749</v>
       </c>
       <c r="E18" s="9">
-        <f>C18+0.667</f>
-        <v>1.5489444444444445</v>
+        <v>0.54893518518518525</v>
       </c>
       <c r="F18" s="9">
         <f t="shared" si="0"/>
-        <v>0.66700000000000004</v>
+        <v>0.66699074074074083</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -1350,7 +1341,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -1375,7 +1366,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -1400,131 +1391,131 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B34" s="8"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B35" s="8"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B36" s="8"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B38" s="8"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B39" s="8"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B42" s="8"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B43" s="8"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B44" s="8"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B45" s="8"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B46" s="8"/>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B47" s="8"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B48" s="8"/>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B49" s="8"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B50" s="8"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B51" s="8"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B52" s="8"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B53" s="8"/>
       <c r="D53" s="8"/>
     </row>
@@ -1541,7 +1532,7 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="7.83203125" customWidth="1"/>
     <col min="2" max="2" width="75" bestFit="1" customWidth="1"/>
@@ -1552,7 +1543,7 @@
     <col min="7" max="7" width="94" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1569,7 +1560,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1593,7 +1584,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1617,7 +1608,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1641,7 +1632,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1665,7 +1656,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1689,7 +1680,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1713,7 +1704,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1737,7 +1728,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1761,7 +1752,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1785,7 +1776,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1809,7 +1800,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1833,7 +1824,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1857,7 +1848,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1881,7 +1872,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1905,7 +1896,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1929,7 +1920,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1953,7 +1944,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1977,7 +1968,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2001,7 +1992,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2026,7 +2017,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2051,7 +2042,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2076,7 +2067,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2101,7 +2092,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2126,7 +2117,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2151,7 +2142,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
     </row>
   </sheetData>
@@ -2164,17 +2155,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF47C328-03B3-8E41-ACAA-74BCC13F52C5}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="3.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B1" s="5" t="s">
         <v>127</v>
       </c>
@@ -2182,7 +2173,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2193,7 +2184,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2204,7 +2195,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2215,7 +2206,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2226,7 +2217,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2237,7 +2228,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2248,7 +2239,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2259,7 +2250,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2270,7 +2261,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2281,7 +2272,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2292,7 +2283,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2303,7 +2294,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2314,7 +2305,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2325,7 +2316,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2336,7 +2327,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2347,7 +2338,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2358,7 +2349,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2369,7 +2360,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2380,7 +2371,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2391,7 +2382,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2402,7 +2393,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2413,7 +2404,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2424,7 +2415,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2435,7 +2426,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2446,7 +2437,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2457,7 +2448,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2468,7 +2459,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2479,7 +2470,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2490,7 +2481,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2501,7 +2492,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2512,7 +2503,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2523,7 +2514,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2534,7 +2525,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2545,7 +2536,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2556,7 +2547,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2567,7 +2558,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
         <v>36</v>
       </c>

</xml_diff>